<commit_message>
Config files:: data source
</commit_message>
<xml_diff>
--- a/Codethon/SyncupEngine/ConfigFiles/Drug.xlsx
+++ b/Codethon/SyncupEngine/ConfigFiles/Drug.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\C402193\Desktop\codeathon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Scrapy\Test\Test\spiders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D270AD8-77EE-4EDF-89F6-DF9B429CB166}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C931F4-1DE9-4212-98C8-0B515D4CF9F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="10980" xr2:uid="{D94ADC51-3DF4-4B2F-B914-5D5E58F55074}"/>
+    <workbookView xWindow="705" yWindow="690" windowWidth="13410" windowHeight="6510" xr2:uid="{D94ADC51-3DF4-4B2F-B914-5D5E58F55074}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Drug Name</t>
   </si>
   <si>
     <t>Aspirin</t>
+  </si>
+  <si>
+    <t>Abreva</t>
   </si>
 </sst>
 </file>
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2771F5F0-79A6-418A-9FCE-8BD389D14AB4}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +403,13 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>